<commit_message>
Tidy up data and image files, as well README.md
</commit_message>
<xml_diff>
--- a/data/raw/abstracts/2020president.xlsx
+++ b/data/raw/abstracts/2020president.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdree\Desktop\GitHub\MSDS696\data\raw\abstracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7AAE2E7-84C5-484F-9154-7E2FA08783B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773C6534-FD2E-477D-ACBE-DED7439F51DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020president" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
-    <t>Biden_ Harris</t>
-  </si>
-  <si>
-    <t>Trump_ Pence</t>
-  </si>
-  <si>
-    <t>Blankenship_ Mohr</t>
-  </si>
-  <si>
     <t>Hammons_Bodenstab</t>
   </si>
   <si>
@@ -281,12 +283,21 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>Biden_Harris</t>
+  </si>
+  <si>
+    <t>Trump_Pence</t>
+  </si>
+  <si>
+    <t>Blankenship_Mohr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1120,11 +1131,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,72 +1163,72 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>134202</v>
@@ -1282,7 +1293,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>3759</v>
@@ -1347,7 +1358,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>213673</v>
@@ -1412,7 +1423,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>3738</v>
@@ -1477,7 +1488,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>317</v>
@@ -1542,7 +1553,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>732</v>
@@ -1607,7 +1618,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>159089</v>
@@ -1672,7 +1683,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>29077</v>
@@ -1737,7 +1748,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>7160</v>
@@ -1802,7 +1813,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>131</v>
@@ -1867,7 +1878,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>3603</v>
@@ -1932,7 +1943,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>1959</v>
@@ -1997,7 +2008,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>1311</v>
@@ -2062,7 +2073,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>437</v>
@@ -2127,7 +2138,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>1111</v>
@@ -2192,7 +2203,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>5887</v>
@@ -2257,7 +2268,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>313292</v>
@@ -2322,7 +2333,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>341</v>
@@ -2387,7 +2398,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>104653</v>
@@ -2452,7 +2463,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>18588</v>
@@ -2517,7 +2528,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>161636</v>
@@ -2582,7 +2593,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>4490</v>
@@ -2647,7 +2658,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>7369</v>
@@ -2712,7 +2723,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <v>15427</v>
@@ -2777,7 +2788,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>2222</v>
@@ -2842,7 +2853,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>4709</v>
@@ -2907,7 +2918,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>6976</v>
@@ -2972,7 +2983,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29">
         <v>255</v>
@@ -3037,7 +3048,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>2076</v>
@@ -3102,7 +3113,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>175</v>
@@ -3167,7 +3178,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>218393</v>
@@ -3232,7 +3243,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>98</v>
@@ -3297,7 +3308,7 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B34">
         <v>662</v>
@@ -3362,7 +3373,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <v>20548</v>
@@ -3427,7 +3438,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B36">
         <v>2303</v>
@@ -3492,7 +3503,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B37">
         <v>126117</v>
@@ -3557,7 +3568,7 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B38">
         <v>3497</v>
@@ -3622,7 +3633,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B39">
         <v>470</v>
@@ -3687,7 +3698,7 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B40">
         <v>2218</v>
@@ -3752,7 +3763,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B41">
         <v>31533</v>
@@ -3817,7 +3828,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B42">
         <v>317</v>
@@ -3882,7 +3893,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B43">
         <v>1203</v>
@@ -3947,7 +3958,7 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B44">
         <v>5836</v>
@@ -4012,7 +4023,7 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B45">
         <v>7687</v>
@@ -4077,7 +4088,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B46">
         <v>3876</v>
@@ -4142,7 +4153,7 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B47">
         <v>3605</v>
@@ -4207,7 +4218,7 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B48">
         <v>2365</v>
@@ -4272,7 +4283,7 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B49">
         <v>4903</v>
@@ -4337,7 +4348,7 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B50">
         <v>486</v>
@@ -4402,7 +4413,7 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B51">
         <v>8989</v>
@@ -4467,7 +4478,7 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B52">
         <v>1458</v>
@@ -4532,7 +4543,7 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B53">
         <v>43772</v>
@@ -4597,7 +4608,7 @@
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B54">
         <v>561</v>
@@ -4662,7 +4673,7 @@
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B55">
         <v>2495</v>
@@ -4727,7 +4738,7 @@
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B56">
         <v>10582</v>
@@ -4792,7 +4803,7 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B57">
         <v>1884</v>
@@ -4857,7 +4868,7 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B58">
         <v>342</v>
@@ -4922,7 +4933,7 @@
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B59">
         <v>3923</v>
@@ -4987,7 +4998,7 @@
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B60">
         <v>301</v>
@@ -5052,7 +5063,7 @@
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B61">
         <v>12620</v>
@@ -5117,7 +5128,7 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B62">
         <v>5278</v>
@@ -5182,7 +5193,7 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B63">
         <v>369</v>
@@ -5247,7 +5258,7 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B64">
         <v>66050</v>
@@ -5312,7 +5323,7 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B65">
         <v>785</v>
@@ -5375,153 +5386,153 @@
         <v>1</v>
       </c>
     </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66">
+        <f>SUM(B2:B65)</f>
+        <v>1803921</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:U66" si="0">SUM(C2:C65)</f>
+        <v>1364202</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>5059</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>2729</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>8981</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>355</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="0"/>
+        <v>52427</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="0"/>
+        <v>2514</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="0"/>
+        <v>568</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="0"/>
+        <v>636</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="0"/>
+        <v>379</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="0"/>
+        <v>762</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="0"/>
+        <v>1035</v>
+      </c>
+      <c r="S66">
+        <f t="shared" si="0"/>
+        <v>614</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="0"/>
+        <v>572</v>
+      </c>
+      <c r="U66">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+    </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B67">
-        <f>SUM(B2:B65)</f>
         <v>1803921</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:U67" si="0">SUM(C2:C65)</f>
         <v>1364202</v>
       </c>
       <c r="D67">
-        <f t="shared" si="0"/>
         <v>5059</v>
       </c>
       <c r="E67">
-        <f t="shared" si="0"/>
         <v>2729</v>
       </c>
       <c r="F67">
-        <f t="shared" si="0"/>
         <v>8981</v>
       </c>
       <c r="G67">
-        <f t="shared" si="0"/>
         <v>355</v>
       </c>
       <c r="H67">
-        <f t="shared" si="0"/>
         <v>52427</v>
       </c>
       <c r="I67">
-        <f t="shared" si="0"/>
         <v>2514</v>
       </c>
       <c r="J67">
-        <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="K67">
-        <f t="shared" si="0"/>
         <v>568</v>
       </c>
       <c r="L67">
-        <f t="shared" si="0"/>
         <v>636</v>
       </c>
       <c r="M67">
-        <f t="shared" si="0"/>
         <v>379</v>
       </c>
       <c r="N67">
-        <f t="shared" si="0"/>
         <v>495</v>
       </c>
       <c r="O67">
-        <f t="shared" si="0"/>
         <v>354</v>
       </c>
       <c r="P67">
-        <f t="shared" si="0"/>
         <v>196</v>
       </c>
       <c r="Q67">
-        <f t="shared" si="0"/>
         <v>762</v>
       </c>
       <c r="R67">
-        <f t="shared" si="0"/>
         <v>1035</v>
       </c>
       <c r="S67">
-        <f t="shared" si="0"/>
         <v>614</v>
       </c>
       <c r="T67">
-        <f t="shared" si="0"/>
         <v>572</v>
       </c>
       <c r="U67">
-        <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68">
-        <v>1803921</v>
-      </c>
-      <c r="C68">
-        <v>1364202</v>
-      </c>
-      <c r="D68">
-        <v>5059</v>
-      </c>
-      <c r="E68">
-        <v>2729</v>
-      </c>
-      <c r="F68">
-        <v>8981</v>
-      </c>
-      <c r="G68">
-        <v>355</v>
-      </c>
-      <c r="H68">
-        <v>52427</v>
-      </c>
-      <c r="I68">
-        <v>2514</v>
-      </c>
-      <c r="J68">
-        <v>2007</v>
-      </c>
-      <c r="K68">
-        <v>568</v>
-      </c>
-      <c r="L68">
-        <v>636</v>
-      </c>
-      <c r="M68">
-        <v>379</v>
-      </c>
-      <c r="N68">
-        <v>495</v>
-      </c>
-      <c r="O68">
-        <v>354</v>
-      </c>
-      <c r="P68">
-        <v>196</v>
-      </c>
-      <c r="Q68">
-        <v>762</v>
-      </c>
-      <c r="R68">
-        <v>1035</v>
-      </c>
-      <c r="S68">
-        <v>614</v>
-      </c>
-      <c r="T68">
-        <v>572</v>
-      </c>
-      <c r="U68">
         <v>175</v>
       </c>
     </row>

</xml_diff>